<commit_message>
QMM008 update template D
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_社会保険事業所一覧.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM008社会保険事業所の登録_社会保険事業所一覧.xlsx
@@ -1262,7 +1262,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1316,9 +1316,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1438,6 +1435,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1473,48 +1512,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -45126,112 +45123,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12" thickBot="1">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
     </row>
     <row r="2" spans="1:14" ht="23.45" customHeight="1" thickTop="1">
-      <c r="A2" s="39"/>
-      <c r="B2" s="43" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="76"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62"/>
     </row>
     <row r="3" spans="1:14" ht="23.45" customHeight="1" thickBot="1">
-      <c r="A3" s="39"/>
-      <c r="B3" s="33" t="s">
+      <c r="A3" s="38"/>
+      <c r="B3" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="65"/>
     </row>
     <row r="4" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A4" s="39"/>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="77"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="79"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="71"/>
     </row>
     <row r="5" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="35" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="73"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="65"/>
     </row>
     <row r="6" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="36" t="s">
+      <c r="A6" s="38"/>
+      <c r="B6" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62" t="s">
+      <c r="E6" s="73"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="77"/>
       <c r="J6" s="6" t="s">
         <v>31</v>
       </c>
@@ -45244,11 +45241,11 @@
       <c r="M6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="40"/>
+      <c r="N6" s="39"/>
     </row>
     <row r="7" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="39"/>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="13"/>
@@ -45261,62 +45258,62 @@
         <v>29</v>
       </c>
       <c r="H7" s="18"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="20" t="s">
+      <c r="I7" s="31"/>
+      <c r="J7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="21" t="s">
+      <c r="K7" s="27"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N7" s="41"/>
+      <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="39"/>
-      <c r="B8" s="38" t="s">
+      <c r="A8" s="38"/>
+      <c r="B8" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="17" t="s">
         <v>30</v>
       </c>
       <c r="H8" s="18"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27" t="s">
+      <c r="I8" s="25"/>
+      <c r="J8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="30"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="42"/>
+      <c r="N8" s="41"/>
     </row>
     <row r="9" spans="1:14" ht="68.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A9" s="39"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="70"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="83"/>
     </row>
     <row r="10" spans="1:14" ht="13.5" thickTop="1" thickBot="1">
       <c r="B10" s="1"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -45328,97 +45325,97 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="23.45" customHeight="1" thickTop="1">
-      <c r="A11" s="39"/>
-      <c r="B11" s="56" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="80"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="82"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="68"/>
     </row>
     <row r="12" spans="1:14" ht="23.45" customHeight="1" thickBot="1">
-      <c r="A12" s="39"/>
-      <c r="B12" s="33" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
-      <c r="N12" s="73"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="65"/>
     </row>
     <row r="13" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A13" s="39"/>
-      <c r="B13" s="34" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="79"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="71"/>
     </row>
     <row r="14" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A14" s="39"/>
-      <c r="B14" s="35" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
-      <c r="M14" s="72"/>
-      <c r="N14" s="73"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="65"/>
     </row>
     <row r="15" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A15" s="39"/>
-      <c r="B15" s="36" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="62" t="s">
+      <c r="E15" s="73"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="63"/>
-      <c r="I15" s="64"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="77"/>
       <c r="J15" s="6" t="s">
         <v>9</v>
       </c>
@@ -45431,11 +45428,11 @@
       <c r="M15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="40"/>
+      <c r="N15" s="39"/>
     </row>
     <row r="16" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="13"/>
@@ -45448,164 +45445,164 @@
         <v>15</v>
       </c>
       <c r="H16" s="18"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="20" t="s">
+      <c r="I16" s="31"/>
+      <c r="J16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="21" t="s">
+      <c r="K16" s="27"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="41"/>
+      <c r="N16" s="40"/>
     </row>
     <row r="17" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A17" s="39"/>
-      <c r="B17" s="38" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="22" t="s">
+      <c r="C17" s="22"/>
+      <c r="D17" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
       <c r="G17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="18"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27" t="s">
+      <c r="I17" s="25"/>
+      <c r="J17" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="31"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="30"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="46"/>
+      <c r="N17" s="45"/>
     </row>
     <row r="18" spans="1:14" ht="68.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="70"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="83"/>
     </row>
     <row r="19" spans="1:14" ht="13.5" thickTop="1" thickBot="1">
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" ht="23.45" customHeight="1" thickTop="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="43" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="74"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="76"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="62"/>
     </row>
     <row r="21" spans="1:14" ht="23.45" customHeight="1" thickBot="1">
-      <c r="A21" s="39"/>
-      <c r="B21" s="33" t="s">
+      <c r="A21" s="38"/>
+      <c r="B21" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
-      <c r="N21" s="73"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="65"/>
     </row>
     <row r="22" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A22" s="39"/>
-      <c r="B22" s="34" t="s">
+      <c r="A22" s="38"/>
+      <c r="B22" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="77"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="78"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="78"/>
-      <c r="M22" s="78"/>
-      <c r="N22" s="79"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+      <c r="L22" s="70"/>
+      <c r="M22" s="70"/>
+      <c r="N22" s="71"/>
     </row>
     <row r="23" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A23" s="39"/>
-      <c r="B23" s="35" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="72"/>
-      <c r="L23" s="72"/>
-      <c r="M23" s="72"/>
-      <c r="N23" s="73"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="65"/>
     </row>
     <row r="24" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="36" t="s">
+      <c r="A24" s="38"/>
+      <c r="B24" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="59" t="s">
+      <c r="D24" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="60"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="62" t="s">
+      <c r="E24" s="73"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="63"/>
-      <c r="I24" s="64"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="77"/>
       <c r="J24" s="6" t="s">
         <v>9</v>
       </c>
@@ -45618,11 +45615,11 @@
       <c r="M24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N24" s="40"/>
+      <c r="N24" s="39"/>
     </row>
     <row r="25" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A25" s="39"/>
-      <c r="B25" s="37" t="s">
+      <c r="A25" s="38"/>
+      <c r="B25" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="13"/>
@@ -45635,69 +45632,62 @@
         <v>15</v>
       </c>
       <c r="H25" s="18"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="20" t="s">
+      <c r="I25" s="31"/>
+      <c r="J25" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="K25" s="28"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="21" t="s">
+      <c r="K25" s="27"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N25" s="41"/>
+      <c r="N25" s="40"/>
     </row>
     <row r="26" spans="1:14" ht="23.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A26" s="39"/>
-      <c r="B26" s="49" t="s">
+      <c r="A26" s="38"/>
+      <c r="B26" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51" t="s">
+      <c r="C26" s="49"/>
+      <c r="D26" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="53"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H26" s="18"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="55" t="s">
+      <c r="I26" s="53"/>
+      <c r="J26" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="83"/>
-      <c r="L26" s="84"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="59"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="42"/>
+      <c r="N26" s="41"/>
     </row>
     <row r="27" spans="1:14" ht="68.45" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A27" s="39"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="66"/>
-      <c r="L27" s="66"/>
-      <c r="M27" s="66"/>
-      <c r="N27" s="67"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="80"/>
     </row>
     <row r="28" spans="1:14" ht="12" thickTop="1">
-      <c r="F28" s="48"/>
+      <c r="F28" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:N3"/>
-    <mergeCell ref="E11:N11"/>
-    <mergeCell ref="E12:N12"/>
-    <mergeCell ref="E13:N13"/>
-    <mergeCell ref="E4:N4"/>
-    <mergeCell ref="E5:N5"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="B27:N27"/>
@@ -45712,6 +45702,13 @@
     <mergeCell ref="E21:N21"/>
     <mergeCell ref="E22:N22"/>
     <mergeCell ref="E23:N23"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="E11:N11"/>
+    <mergeCell ref="E12:N12"/>
+    <mergeCell ref="E13:N13"/>
+    <mergeCell ref="E4:N4"/>
+    <mergeCell ref="E5:N5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>